<commit_message>
check all transcripts and rerun pre-processing
</commit_message>
<xml_diff>
--- a/data/expt_2/raw_transcripts/game41.xlsx
+++ b/data/expt_2/raw_transcripts/game41.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="MVI_0065.MP4.csv" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="MVI_0065.MP4.csv" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>Unknown Author</author>
   </authors>
   <commentList>
     <comment ref="C143" authorId="0">
@@ -30,10 +30,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">child made head movements to show this one
 	-Rebecca Jacqueline Pizzitola</t>
@@ -45,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="197">
   <si>
     <t xml:space="preserve">start</t>
   </si>
@@ -482,12 +480,15 @@
     <t xml:space="preserve">Human.</t>
   </si>
   <si>
-    <t xml:space="preserve">human, standing human</t>
+    <t xml:space="preserve">human</t>
   </si>
   <si>
     <t xml:space="preserve">Standing human.</t>
   </si>
   <si>
+    <t xml:space="preserve">standing human</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Now you are the guesser, [pear444] and you're the teller, [apple333].</t>
   </si>
   <si>
@@ -536,12 +537,15 @@
     <t xml:space="preserve">Stand up and eyes down.</t>
   </si>
   <si>
-    <t xml:space="preserve">stand up and eyes down walking human</t>
+    <t xml:space="preserve">stand up and eyes down</t>
   </si>
   <si>
     <t xml:space="preserve">Walking human.</t>
   </si>
   <si>
+    <t xml:space="preserve">walking human</t>
+  </si>
+  <si>
     <t xml:space="preserve"> This time, only tell me one, ten, sta- standing.</t>
   </si>
   <si>
@@ -557,7 +561,7 @@
     <t xml:space="preserve">Walking and head down and eyes down.</t>
   </si>
   <si>
-    <t xml:space="preserve">walking and head down and eyes down, walking human</t>
+    <t xml:space="preserve">walking and head down and eyes down</t>
   </si>
   <si>
     <t xml:space="preserve">walking human.</t>
@@ -587,10 +591,13 @@
     <t xml:space="preserve">Human with head up.</t>
   </si>
   <si>
-    <t xml:space="preserve">human with head up with eyes</t>
+    <t xml:space="preserve">human with head up</t>
   </si>
   <si>
     <t xml:space="preserve">With eyes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with eyes</t>
   </si>
   <si>
     <t xml:space="preserve"> with eyes, with eyes.</t>
@@ -636,7 +643,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -665,6 +672,11 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -709,12 +721,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -730,2939 +750,3055 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H188"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F146" activeCellId="0" sqref="F146"/>
+      <selection pane="bottomLeft" activeCell="E188" activeCellId="0" sqref="E188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>3000</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>3000</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>8000</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>8000</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>13000</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>13000</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>15000</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>15000</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>20000</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>20000</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <v>21000</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>21000</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="2" t="n">
         <v>22000</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>22000</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="2" t="n">
         <v>24000</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="2" t="n">
         <v>24000</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="2" t="n">
         <v>27000</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="2" t="n">
         <v>27000</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="2" t="n">
         <v>30000</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="2" t="n">
         <v>30000</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="2" t="n">
         <v>30840</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="2" t="n">
         <v>30840</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="2" t="n">
         <v>32080</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="2" t="n">
         <v>32080</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="2" t="n">
         <v>32840</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="2" t="n">
         <v>35800</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="2" t="n">
         <v>37480</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="2" t="n">
         <v>37480</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="2" t="n">
         <v>38500</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="2" t="n">
         <v>38500</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="B17" s="2" t="n">
         <v>39160</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="2" t="n">
         <v>40320</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="B18" s="2" t="n">
         <v>42760</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="2" t="n">
         <v>42760</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="B19" s="2" t="n">
         <v>45320</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="2" t="n">
         <v>47280</v>
       </c>
-      <c r="B20" s="1" t="n">
+      <c r="B20" s="2" t="n">
         <v>48320</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="2" t="n">
         <v>48320</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="2" t="n">
         <v>49320</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="2" t="n">
         <v>51800</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" s="2" t="n">
         <v>53920</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="2" t="n">
         <v>55780</v>
       </c>
-      <c r="B23" s="1" t="n">
+      <c r="B23" s="2" t="n">
         <v>57380</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="2" t="n">
         <v>57380</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="B24" s="2" t="n">
         <v>58540</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="2" t="n">
         <v>58540</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="2" t="n">
         <v>59740</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="2" t="n">
         <v>59740</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="B26" s="2" t="n">
         <v>61380</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="2" t="n">
         <v>61380</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="B27" s="2" t="n">
         <v>64620</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="2" t="n">
         <v>64620</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="2" t="n">
         <v>67480</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="2" t="n">
         <v>67480</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="B29" s="2" t="n">
         <v>68880</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
+      <c r="A30" s="2" t="n">
         <v>68880</v>
       </c>
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="2" t="n">
         <v>70360</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+      <c r="A31" s="2" t="n">
         <v>70360</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="2" t="n">
         <v>71660</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="2" t="n">
         <v>71660</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="2" t="n">
         <v>72360</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="2" t="n">
         <v>72360</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="2" t="n">
         <v>73260</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+      <c r="A34" s="2" t="n">
         <v>73260</v>
       </c>
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="2" t="n">
         <v>75160</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="2" t="n">
         <v>75160</v>
       </c>
-      <c r="B35" s="1" t="n">
+      <c r="B35" s="2" t="n">
         <v>75520</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
+      <c r="A36" s="2" t="n">
         <v>75520</v>
       </c>
-      <c r="B36" s="1" t="n">
+      <c r="B36" s="2" t="n">
         <v>77300</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+      <c r="A37" s="2" t="n">
         <v>77300</v>
       </c>
-      <c r="B37" s="1" t="n">
+      <c r="B37" s="2" t="n">
         <v>78620</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
+      <c r="A38" s="2" t="n">
         <v>78620</v>
       </c>
-      <c r="B38" s="1" t="n">
+      <c r="B38" s="2" t="n">
         <v>79620</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+      <c r="A39" s="2" t="n">
         <v>79620</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="2" t="n">
         <v>80460</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="2" t="n">
         <v>80460</v>
       </c>
-      <c r="B40" s="1" t="n">
+      <c r="B40" s="2" t="n">
         <v>81540</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="2" t="n">
         <v>81540</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="B41" s="2" t="n">
         <v>82200</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
+      <c r="A42" s="2" t="n">
         <v>82200</v>
       </c>
-      <c r="B42" s="1" t="n">
+      <c r="B42" s="2" t="n">
         <v>83660</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
+      <c r="A43" s="2" t="n">
         <v>83660</v>
       </c>
-      <c r="B43" s="1" t="n">
+      <c r="B43" s="2" t="n">
         <v>85180</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
+      <c r="A44" s="2" t="n">
         <v>85180</v>
       </c>
-      <c r="B44" s="1" t="n">
+      <c r="B44" s="2" t="n">
         <v>87340</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
+      <c r="A45" s="2" t="n">
         <v>87340</v>
       </c>
-      <c r="B45" s="1" t="n">
+      <c r="B45" s="2" t="n">
         <v>89140</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
+      <c r="A46" s="2" t="n">
         <v>89140</v>
       </c>
-      <c r="B46" s="1" t="n">
+      <c r="B46" s="2" t="n">
         <v>91800</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+      <c r="A47" s="2" t="n">
         <v>91800</v>
       </c>
-      <c r="B47" s="1" t="n">
+      <c r="B47" s="2" t="n">
         <v>97660</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
+      <c r="A48" s="2" t="n">
         <v>97660</v>
       </c>
-      <c r="B48" s="1" t="n">
+      <c r="B48" s="2" t="n">
         <v>100080</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
+      <c r="A49" s="2" t="n">
         <v>100080</v>
       </c>
-      <c r="B49" s="1" t="n">
+      <c r="B49" s="2" t="n">
         <v>102580</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
+      <c r="A50" s="2" t="n">
         <v>102580</v>
       </c>
-      <c r="B50" s="1" t="n">
+      <c r="B50" s="2" t="n">
         <v>105500</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
+      <c r="A51" s="2" t="n">
         <v>105500</v>
       </c>
-      <c r="B51" s="1" t="n">
+      <c r="B51" s="2" t="n">
         <v>107200</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
+      <c r="A52" s="2" t="n">
         <v>107200</v>
       </c>
-      <c r="B52" s="1" t="n">
+      <c r="B52" s="2" t="n">
         <v>109280</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
+      <c r="A53" s="2" t="n">
         <v>109280</v>
       </c>
-      <c r="B53" s="1" t="n">
+      <c r="B53" s="2" t="n">
         <v>112240</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
+      <c r="A54" s="2" t="n">
         <v>112240</v>
       </c>
-      <c r="B54" s="1" t="n">
+      <c r="B54" s="2" t="n">
         <v>113080</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="2" t="n">
         <v>113080</v>
       </c>
-      <c r="B55" s="1" t="n">
+      <c r="B55" s="2" t="n">
         <v>114560</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="2" t="n">
         <v>114560</v>
       </c>
-      <c r="B56" s="1" t="n">
+      <c r="B56" s="2" t="n">
         <v>115840</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="2" t="n">
         <v>115840</v>
       </c>
-      <c r="B57" s="1" t="n">
+      <c r="B57" s="2" t="n">
         <v>117980</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="2" t="n">
         <v>117980</v>
       </c>
-      <c r="B58" s="1" t="n">
+      <c r="B58" s="2" t="n">
         <v>120960</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="2" t="n">
         <v>120960</v>
       </c>
-      <c r="B59" s="1" t="n">
+      <c r="B59" s="2" t="n">
         <v>122460</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="2" t="n">
         <v>122460</v>
       </c>
-      <c r="B60" s="1" t="n">
+      <c r="B60" s="2" t="n">
         <v>125760</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="2" t="n">
         <v>125760</v>
       </c>
-      <c r="B61" s="1" t="n">
+      <c r="B61" s="2" t="n">
         <v>129860</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="2" t="n">
         <v>129860</v>
       </c>
-      <c r="B62" s="1" t="n">
+      <c r="B62" s="2" t="n">
         <v>132280</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="2" t="n">
         <v>132280</v>
       </c>
-      <c r="B63" s="1" t="n">
+      <c r="B63" s="2" t="n">
         <v>134340</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="2" t="n">
         <v>134340</v>
       </c>
-      <c r="B64" s="1" t="n">
+      <c r="B64" s="2" t="n">
         <v>136860</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="2" t="n">
         <v>136860</v>
       </c>
-      <c r="B65" s="1" t="n">
+      <c r="B65" s="2" t="n">
         <v>140420</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="2" t="n">
         <v>140420</v>
       </c>
-      <c r="B66" s="1" t="n">
+      <c r="B66" s="2" t="n">
         <v>141700</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="n">
+      <c r="A67" s="2" t="n">
         <v>141700</v>
       </c>
-      <c r="B67" s="1" t="n">
+      <c r="B67" s="2" t="n">
         <v>143740</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="n">
+      <c r="A68" s="2" t="n">
         <v>143740</v>
       </c>
-      <c r="B68" s="1" t="n">
+      <c r="B68" s="2" t="n">
         <v>145840</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="n">
+      <c r="A69" s="2" t="n">
         <v>147180</v>
       </c>
-      <c r="B69" s="1" t="n">
+      <c r="B69" s="2" t="n">
         <v>148180</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E69" s="1" t="n">
+      <c r="E69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F69" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="n">
+      <c r="A70" s="2" t="n">
         <v>148280</v>
       </c>
-      <c r="B70" s="1" t="n">
+      <c r="B70" s="2" t="n">
         <v>149420</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="n">
+      <c r="A71" s="2" t="n">
         <v>149520</v>
       </c>
-      <c r="B71" s="1" t="n">
+      <c r="B71" s="2" t="n">
         <v>150460</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
+      <c r="A72" s="2" t="n">
         <v>151000</v>
       </c>
-      <c r="B72" s="1" t="n">
+      <c r="B72" s="2" t="n">
         <v>152660</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="F72" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="n">
+      <c r="A73" s="2" t="n">
         <v>152760</v>
       </c>
-      <c r="B73" s="1" t="n">
+      <c r="B73" s="2" t="n">
         <v>153260</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="n">
+      <c r="A74" s="2" t="n">
         <v>153420</v>
       </c>
-      <c r="B74" s="1" t="n">
+      <c r="B74" s="2" t="n">
         <v>156680</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
+      <c r="A75" s="2" t="n">
         <v>157240</v>
       </c>
-      <c r="B75" s="1" t="n">
+      <c r="B75" s="2" t="n">
         <v>158400</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="n">
+      <c r="A76" s="2" t="n">
         <v>158600</v>
       </c>
-      <c r="B76" s="1" t="n">
+      <c r="B76" s="2" t="n">
         <v>162700</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="n">
+      <c r="A77" s="2" t="n">
         <v>163240</v>
       </c>
-      <c r="B77" s="1" t="n">
+      <c r="B77" s="2" t="n">
         <v>163620</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F77" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H77" s="1" t="s">
+      <c r="H77" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="n">
+      <c r="A78" s="2" t="n">
         <v>164240</v>
       </c>
-      <c r="B78" s="1" t="n">
+      <c r="B78" s="2" t="n">
         <v>164640</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="F78" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H78" s="1" t="s">
+      <c r="H78" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
+      <c r="A79" s="2" t="n">
         <v>165200</v>
       </c>
-      <c r="B79" s="1" t="n">
+      <c r="B79" s="2" t="n">
         <v>166200</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="n">
+      <c r="A80" s="2" t="n">
         <v>166200</v>
       </c>
-      <c r="B80" s="1" t="n">
+      <c r="B80" s="2" t="n">
         <v>168200</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F80" s="1" t="s">
+      <c r="F80" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="n">
+      <c r="A81" s="2" t="n">
         <v>168200</v>
       </c>
-      <c r="B81" s="1" t="n">
+      <c r="B81" s="2" t="n">
         <v>169200</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="n">
+      <c r="A82" s="2" t="n">
         <v>169200</v>
       </c>
-      <c r="B82" s="1" t="n">
+      <c r="B82" s="2" t="n">
         <v>172200</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="n">
+      <c r="A83" s="2" t="n">
         <v>172200</v>
       </c>
-      <c r="B83" s="1" t="n">
+      <c r="B83" s="2" t="n">
         <v>177200</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="n">
+      <c r="A84" s="2" t="n">
         <v>177200</v>
       </c>
-      <c r="B84" s="1" t="n">
+      <c r="B84" s="2" t="n">
         <v>178200</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E84" s="1" t="n">
+      <c r="E84" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F84" s="1" t="s">
+      <c r="F84" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H84" s="1" t="s">
+      <c r="H84" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="n">
+      <c r="A85" s="2" t="n">
         <v>178200</v>
       </c>
-      <c r="B85" s="1" t="n">
+      <c r="B85" s="2" t="n">
         <v>183200</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D85" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
+      <c r="A86" s="2" t="n">
         <v>183200</v>
       </c>
-      <c r="B86" s="1" t="n">
+      <c r="B86" s="2" t="n">
         <v>187200</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D86" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
+      <c r="A87" s="2" t="n">
         <v>187200</v>
       </c>
-      <c r="B87" s="1" t="n">
+      <c r="B87" s="2" t="n">
         <v>189200</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D87" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E87" s="1" t="n">
+      <c r="E87" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F87" s="1" t="s">
+      <c r="F87" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H87" s="1" t="s">
+      <c r="H87" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="n">
+      <c r="A88" s="2" t="n">
         <v>189200</v>
       </c>
-      <c r="B88" s="1" t="n">
+      <c r="B88" s="2" t="n">
         <v>191200</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F88" s="1" t="s">
+      <c r="F88" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H88" s="1" t="s">
+      <c r="H88" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="n">
+      <c r="A89" s="2" t="n">
         <v>191200</v>
       </c>
-      <c r="B89" s="1" t="n">
+      <c r="B89" s="2" t="n">
         <v>195200</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="n">
+      <c r="A90" s="2" t="n">
         <v>195200</v>
       </c>
-      <c r="B90" s="1" t="n">
+      <c r="B90" s="2" t="n">
         <v>200840</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="n">
+      <c r="A91" s="2" t="n">
         <v>201440</v>
       </c>
-      <c r="B91" s="1" t="n">
+      <c r="B91" s="2" t="n">
         <v>206220</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="n">
+      <c r="A92" s="2" t="n">
         <v>201440</v>
       </c>
-      <c r="B92" s="1" t="n">
+      <c r="B92" s="2" t="n">
         <v>206220</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D92" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E92" s="1" t="n">
+      <c r="E92" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="F92" s="1" t="s">
+      <c r="F92" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H92" s="1" t="s">
+      <c r="H92" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="n">
+      <c r="A93" s="2" t="n">
         <v>209120</v>
       </c>
-      <c r="B93" s="1" t="n">
+      <c r="B93" s="2" t="n">
         <v>216460</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D93" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="n">
+      <c r="A94" s="2" t="n">
         <v>216460</v>
       </c>
-      <c r="B94" s="1" t="n">
+      <c r="B94" s="2" t="n">
         <v>217460</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E94" s="1" t="n">
+      <c r="E94" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F94" s="1" t="s">
+      <c r="F94" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H94" s="1" t="s">
+      <c r="H94" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="n">
+      <c r="A95" s="2" t="n">
         <v>217460</v>
       </c>
-      <c r="B95" s="1" t="n">
+      <c r="B95" s="2" t="n">
         <v>218460</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D95" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="n">
+      <c r="A96" s="2" t="n">
         <v>218460</v>
       </c>
-      <c r="B96" s="1" t="n">
+      <c r="B96" s="2" t="n">
         <v>220460</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D96" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="n">
+      <c r="A97" s="2" t="n">
         <v>220460</v>
       </c>
-      <c r="B97" s="1" t="n">
+      <c r="B97" s="2" t="n">
         <v>221460</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D97" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="n">
+      <c r="A98" s="2" t="n">
         <v>221460</v>
       </c>
-      <c r="B98" s="1" t="n">
+      <c r="B98" s="2" t="n">
         <v>225460</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D98" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="n">
+      <c r="A99" s="2" t="n">
         <v>225460</v>
       </c>
-      <c r="B99" s="1" t="n">
+      <c r="B99" s="2" t="n">
         <v>227460</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D99" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E99" s="1" t="n">
+      <c r="E99" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F99" s="1" t="s">
+      <c r="F99" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H99" s="1" t="s">
+      <c r="H99" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="n">
+      <c r="A100" s="2" t="n">
         <v>227460</v>
       </c>
-      <c r="B100" s="1" t="n">
+      <c r="B100" s="2" t="n">
         <v>228460</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D100" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="n">
+      <c r="A101" s="2" t="n">
         <v>228460</v>
       </c>
-      <c r="B101" s="1" t="n">
+      <c r="B101" s="2" t="n">
         <v>229460</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D101" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="1" t="n">
+      <c r="A102" s="2" t="n">
         <v>229460</v>
       </c>
-      <c r="B102" s="1" t="n">
+      <c r="B102" s="2" t="n">
         <v>232460</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D102" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="1" t="n">
+      <c r="A103" s="2" t="n">
         <v>232460</v>
       </c>
-      <c r="B103" s="1" t="n">
+      <c r="B103" s="2" t="n">
         <v>234460</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="n">
+      <c r="A104" s="2" t="n">
         <v>234460</v>
       </c>
-      <c r="B104" s="1" t="n">
+      <c r="B104" s="2" t="n">
         <v>235460</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="n">
+      <c r="A105" s="2" t="n">
         <v>235460</v>
       </c>
-      <c r="B105" s="1" t="n">
+      <c r="B105" s="2" t="n">
         <v>236460</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="1" t="n">
+      <c r="A106" s="2" t="n">
         <v>236460</v>
       </c>
-      <c r="B106" s="1" t="n">
+      <c r="B106" s="2" t="n">
         <v>238460</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D106" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="n">
+      <c r="A107" s="2" t="n">
         <v>238460</v>
       </c>
-      <c r="B107" s="1" t="n">
+      <c r="B107" s="2" t="n">
         <v>239460</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D107" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="1" t="n">
+      <c r="A108" s="2" t="n">
         <v>239460</v>
       </c>
-      <c r="B108" s="1" t="n">
+      <c r="B108" s="2" t="n">
         <v>240460</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D108" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E108" s="1" t="n">
+      <c r="E108" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="F108" s="1" t="s">
+      <c r="F108" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="1" t="n">
+      <c r="A109" s="2" t="n">
         <v>240460</v>
       </c>
-      <c r="B109" s="1" t="n">
+      <c r="B109" s="2" t="n">
         <v>242460</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D109" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="n">
+      <c r="A110" s="2" t="n">
         <v>242460</v>
       </c>
-      <c r="B110" s="1" t="n">
+      <c r="B110" s="2" t="n">
         <v>243460</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D110" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F110" s="1" t="s">
+      <c r="F110" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H110" s="1" t="s">
+      <c r="H110" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="n">
+      <c r="A111" s="2" t="n">
         <v>243460</v>
       </c>
-      <c r="B111" s="1" t="n">
+      <c r="B111" s="2" t="n">
         <v>244460</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D111" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F111" s="1" t="s">
+      <c r="F111" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1" t="n">
+      <c r="A112" s="2" t="n">
         <v>244460</v>
       </c>
-      <c r="B112" s="1" t="n">
+      <c r="B112" s="2" t="n">
         <v>246460</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D112" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F112" s="1" t="s">
+      <c r="F112" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H112" s="1" t="s">
+      <c r="H112" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="n">
+      <c r="A113" s="2" t="n">
         <v>246460</v>
       </c>
-      <c r="B113" s="1" t="n">
+      <c r="B113" s="2" t="n">
         <v>248460</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D113" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F113" s="1" t="s">
+      <c r="F113" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="n">
+      <c r="A114" s="2" t="n">
         <v>248460</v>
       </c>
-      <c r="B114" s="1" t="n">
+      <c r="B114" s="2" t="n">
         <v>249460</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D114" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="n">
+      <c r="A115" s="2" t="n">
         <v>249460</v>
       </c>
-      <c r="B115" s="1" t="n">
+      <c r="B115" s="2" t="n">
         <v>251460</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D115" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="1" t="n">
+      <c r="A116" s="2" t="n">
         <v>251460</v>
       </c>
-      <c r="B116" s="1" t="n">
+      <c r="B116" s="2" t="n">
         <v>252460</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D116" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F116" s="1" t="s">
+      <c r="F116" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="n">
+      <c r="A117" s="2" t="n">
         <v>252460</v>
       </c>
-      <c r="B117" s="1" t="n">
+      <c r="B117" s="2" t="n">
         <v>253460</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D117" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F117" s="1" t="s">
+      <c r="F117" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="n">
+      <c r="A118" s="2" t="n">
         <v>254460</v>
       </c>
-      <c r="B118" s="1" t="n">
+      <c r="B118" s="2" t="n">
         <v>257460</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D118" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="n">
+      <c r="A119" s="2" t="n">
         <v>257460</v>
       </c>
-      <c r="B119" s="1" t="n">
+      <c r="B119" s="2" t="n">
         <v>261460</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D119" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="n">
+      <c r="A120" s="2" t="n">
         <v>261460</v>
       </c>
-      <c r="B120" s="1" t="n">
+      <c r="B120" s="2" t="n">
         <v>262460</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D120" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="n">
+      <c r="A121" s="2" t="n">
         <v>262460</v>
       </c>
-      <c r="B121" s="1" t="n">
+      <c r="B121" s="2" t="n">
         <v>267460</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D121" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="n">
+      <c r="A122" s="2" t="n">
         <v>262460</v>
       </c>
-      <c r="B122" s="1" t="n">
+      <c r="B122" s="2" t="n">
         <v>267460</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D122" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E122" s="1" t="n">
+      <c r="E122" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="F122" s="1" t="s">
+      <c r="F122" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H122" s="1" t="s">
+      <c r="H122" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="n">
+      <c r="A123" s="2" t="n">
         <v>267460</v>
       </c>
-      <c r="B123" s="1" t="n">
+      <c r="B123" s="2" t="n">
         <v>276460</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C123" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D123" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="1" t="n">
+      <c r="A124" s="2" t="n">
         <v>267460</v>
       </c>
-      <c r="B124" s="1" t="n">
+      <c r="B124" s="2" t="n">
         <v>276460</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C124" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D124" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F124" s="1" t="s">
+      <c r="F124" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1" t="n">
+      <c r="A125" s="2" t="n">
         <v>276460</v>
       </c>
-      <c r="B125" s="1" t="n">
+      <c r="B125" s="2" t="n">
         <v>280460</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D125" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="n">
+      <c r="A126" s="2" t="n">
         <v>280460</v>
       </c>
-      <c r="B126" s="1" t="n">
+      <c r="B126" s="2" t="n">
         <v>283460</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C126" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="D126" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E126" s="1" t="n">
+      <c r="E126" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="F126" s="1" t="s">
+      <c r="F126" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H126" s="1" t="s">
+      <c r="H126" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1" t="n">
+      <c r="A127" s="2" t="n">
         <v>280460</v>
       </c>
-      <c r="B127" s="1" t="n">
+      <c r="B127" s="2" t="n">
         <v>283460</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="D127" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F127" s="1" t="s">
+      <c r="F127" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="1" t="n">
+      <c r="A128" s="2" t="n">
         <v>283460</v>
       </c>
-      <c r="B128" s="1" t="n">
+      <c r="B128" s="2" t="n">
         <v>290960</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C128" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="D128" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="1" t="n">
+      <c r="A129" s="2" t="n">
         <v>290960</v>
       </c>
-      <c r="B129" s="1" t="n">
+      <c r="B129" s="2" t="n">
         <v>291960</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C129" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="D129" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="n">
+      <c r="A130" s="2" t="n">
         <v>291960</v>
       </c>
-      <c r="B130" s="1" t="n">
+      <c r="B130" s="2" t="n">
         <v>292960</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C130" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="D130" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E130" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="F130" s="1" t="s">
+      <c r="E130" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="F130" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H130" s="1" t="s">
+      <c r="H130" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="n">
+      <c r="A131" s="2" t="n">
         <v>292960</v>
       </c>
-      <c r="B131" s="1" t="n">
+      <c r="B131" s="2" t="n">
         <v>293960</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C131" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D131" s="1" t="s">
+      <c r="D131" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F131" s="1" t="s">
+      <c r="F131" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="H131" s="3" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="n">
+      <c r="A132" s="2" t="n">
         <v>293960</v>
       </c>
-      <c r="B132" s="1" t="n">
+      <c r="B132" s="2" t="n">
         <v>294960</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="C132" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="D132" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="n">
+      <c r="A133" s="2" t="n">
         <v>294960</v>
       </c>
-      <c r="B133" s="1" t="n">
+      <c r="B133" s="2" t="n">
         <v>295960</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="C133" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D133" s="1" t="s">
+      <c r="D133" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1" t="n">
+      <c r="A134" s="2" t="n">
         <v>295960</v>
       </c>
-      <c r="B134" s="1" t="n">
+      <c r="B134" s="2" t="n">
         <v>296960</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C134" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="D134" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="n">
+      <c r="A135" s="2" t="n">
         <v>296960</v>
       </c>
-      <c r="B135" s="1" t="n">
+      <c r="B135" s="2" t="n">
         <v>301960</v>
       </c>
-      <c r="C135" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D135" s="1" t="s">
+      <c r="C135" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D135" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="n">
+      <c r="A136" s="2" t="n">
         <v>301960</v>
       </c>
-      <c r="B136" s="1" t="n">
+      <c r="B136" s="2" t="n">
         <v>303960</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D136" s="1" t="s">
+      <c r="C136" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D136" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E136" s="1" t="n">
+      <c r="E136" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F136" s="1" t="s">
+      <c r="F136" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H136" s="1" t="s">
+      <c r="H136" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="n">
+      <c r="A137" s="2" t="n">
         <v>303960</v>
       </c>
-      <c r="B137" s="1" t="n">
+      <c r="B137" s="2" t="n">
         <v>304960</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C137" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="D137" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="n">
+      <c r="A138" s="2" t="n">
         <v>304960</v>
       </c>
-      <c r="B138" s="1" t="n">
+      <c r="B138" s="2" t="n">
         <v>305960</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="C138" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="D138" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="n">
+      <c r="A139" s="2" t="n">
         <v>305960</v>
       </c>
-      <c r="B139" s="1" t="n">
+      <c r="B139" s="2" t="n">
         <v>307960</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C139" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="D139" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="n">
+      <c r="A140" s="2" t="n">
         <v>307960</v>
       </c>
-      <c r="B140" s="1" t="n">
+      <c r="B140" s="2" t="n">
         <v>310960</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D140" s="1" t="s">
+      <c r="C140" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D140" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F140" s="1" t="s">
+      <c r="F140" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="n">
+      <c r="A141" s="2" t="n">
         <v>310960</v>
       </c>
-      <c r="B141" s="1" t="n">
+      <c r="B141" s="2" t="n">
         <v>312960</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D141" s="1" t="s">
+      <c r="C141" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D141" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="n">
+      <c r="A142" s="2" t="n">
         <v>312960</v>
       </c>
-      <c r="B142" s="1" t="n">
+      <c r="B142" s="2" t="n">
         <v>315960</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D142" s="1" t="s">
+      <c r="C142" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D142" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="n">
+      <c r="A143" s="2" t="n">
         <v>315960</v>
       </c>
-      <c r="B143" s="1" t="n">
+      <c r="B143" s="2" t="n">
         <v>318960</v>
       </c>
-      <c r="C143" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D143" s="1" t="s">
+      <c r="C143" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D143" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E143" s="1" t="n">
+      <c r="E143" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="F143" s="1" t="s">
+      <c r="F143" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H143" s="1" t="s">
-        <v>153</v>
+      <c r="H143" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="n">
+      <c r="A144" s="2" t="n">
         <v>318960</v>
       </c>
-      <c r="B144" s="1" t="n">
+      <c r="B144" s="2" t="n">
         <v>319960</v>
       </c>
-      <c r="C144" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D144" s="1" t="s">
+      <c r="C144" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D144" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E144" s="1"/>
-      <c r="F144" s="0" t="s">
+      <c r="E144" s="2"/>
+      <c r="F144" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="n">
+      <c r="A145" s="2" t="n">
         <v>321960</v>
       </c>
-      <c r="B145" s="1" t="n">
+      <c r="B145" s="2" t="n">
         <v>322960</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="C145" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D145" s="1" t="s">
+      <c r="D145" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="n">
+      <c r="A146" s="2" t="n">
         <v>322960</v>
       </c>
-      <c r="B146" s="1" t="n">
+      <c r="B146" s="2" t="n">
         <v>328960</v>
       </c>
-      <c r="C146" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D146" s="1" t="s">
+      <c r="C146" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D146" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="1" t="n">
+      <c r="A147" s="2" t="n">
         <v>328960</v>
       </c>
-      <c r="B147" s="1" t="n">
+      <c r="B147" s="2" t="n">
         <v>330960</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C147" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="D147" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E147" s="1" t="n">
+      <c r="E147" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="F147" s="1" t="s">
+      <c r="F147" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H147" s="1" t="s">
+      <c r="H147" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="1" t="n">
+      <c r="A148" s="2" t="n">
         <v>330960</v>
       </c>
-      <c r="B148" s="1" t="n">
+      <c r="B148" s="2" t="n">
         <v>331960</v>
       </c>
-      <c r="C148" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D148" s="1" t="s">
+      <c r="C148" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D148" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="1" t="n">
+      <c r="A149" s="2" t="n">
         <v>331960</v>
       </c>
-      <c r="B149" s="1" t="n">
+      <c r="B149" s="2" t="n">
         <v>333960</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C149" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D149" s="1" t="s">
+      <c r="D149" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="n">
+      <c r="A150" s="2" t="n">
         <v>333960</v>
       </c>
-      <c r="B150" s="1" t="n">
+      <c r="B150" s="2" t="n">
         <v>336960</v>
       </c>
-      <c r="C150" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D150" s="1" t="s">
+      <c r="C150" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D150" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="n">
+      <c r="A151" s="2" t="n">
         <v>336960</v>
       </c>
-      <c r="B151" s="1" t="n">
+      <c r="B151" s="2" t="n">
         <v>338960</v>
       </c>
-      <c r="C151" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D151" s="1" t="s">
+      <c r="C151" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D151" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E151" s="1" t="n">
+      <c r="E151" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="F151" s="1" t="s">
+      <c r="F151" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H151" s="1" t="s">
-        <v>159</v>
+      <c r="H151" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="1" t="n">
+      <c r="A152" s="2" t="n">
         <v>338960</v>
       </c>
-      <c r="B152" s="1" t="n">
+      <c r="B152" s="2" t="n">
         <v>340960</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C152" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D152" s="1" t="s">
+      <c r="D152" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="1" t="n">
+      <c r="A153" s="2" t="n">
         <v>340960</v>
       </c>
-      <c r="B153" s="1" t="n">
+      <c r="B153" s="2" t="n">
         <v>343960</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C153" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="2" t="n">
+        <v>343960</v>
+      </c>
+      <c r="B154" s="2" t="n">
+        <v>346960</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="2" t="n">
+        <v>346960</v>
+      </c>
+      <c r="B155" s="2" t="n">
+        <v>349960</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E155" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H155" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="2" t="n">
+        <v>351960</v>
+      </c>
+      <c r="B156" s="2" t="n">
+        <v>353960</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H156" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="2" t="n">
+        <v>353960</v>
+      </c>
+      <c r="B157" s="2" t="n">
+        <v>355960</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="2" t="n">
+        <v>355960</v>
+      </c>
+      <c r="B158" s="2" t="n">
+        <v>359960</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E158" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H158" s="2"/>
+    </row>
+    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="2" t="n">
+        <v>359960</v>
+      </c>
+      <c r="B159" s="2" t="n">
+        <v>361960</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="2" t="n">
+        <v>361960</v>
+      </c>
+      <c r="B160" s="2" t="n">
+        <v>364960</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="2" t="n">
+        <v>364960</v>
+      </c>
+      <c r="B161" s="2" t="n">
+        <v>365960</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H161" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="2" t="n">
+        <v>367960</v>
+      </c>
+      <c r="B162" s="2" t="n">
+        <v>371960</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="2" t="n">
+        <v>371960</v>
+      </c>
+      <c r="B163" s="2" t="n">
+        <v>375960</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E163" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H163" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="2" t="n">
+        <v>375960</v>
+      </c>
+      <c r="B164" s="2" t="n">
+        <v>379960</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F164" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H164" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="2" t="n">
+        <v>379960</v>
+      </c>
+      <c r="B165" s="2" t="n">
+        <v>382960</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F165" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="2" t="n">
+        <v>382960</v>
+      </c>
+      <c r="B166" s="2" t="n">
+        <v>383960</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F166" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="2" t="n">
+        <v>383960</v>
+      </c>
+      <c r="B167" s="2" t="n">
+        <v>385960</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F167" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="2" t="n">
+        <v>385960</v>
+      </c>
+      <c r="B168" s="2" t="n">
+        <v>386960</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F168" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="2" t="n">
+        <v>386960</v>
+      </c>
+      <c r="B169" s="2" t="n">
+        <v>387960</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F169" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="2" t="n">
+        <v>387960</v>
+      </c>
+      <c r="B170" s="2" t="n">
+        <v>392960</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="2" t="n">
+        <v>392960</v>
+      </c>
+      <c r="B171" s="2" t="n">
+        <v>395960</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="2" t="n">
+        <v>395960</v>
+      </c>
+      <c r="B172" s="2" t="n">
+        <v>397960</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="2" t="n">
+        <v>397960</v>
+      </c>
+      <c r="B173" s="2" t="n">
+        <v>401960</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E173" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="F173" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H173" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="2" t="n">
+        <v>401960</v>
+      </c>
+      <c r="B174" s="2" t="n">
+        <v>404960</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F174" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H174" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="2" t="n">
+        <v>404960</v>
+      </c>
+      <c r="B175" s="2" t="n">
+        <v>407960</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D175" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F175" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="2" t="n">
+        <v>407960</v>
+      </c>
+      <c r="B176" s="2" t="n">
+        <v>410960</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="2" t="n">
+        <v>410960</v>
+      </c>
+      <c r="B177" s="2" t="n">
+        <v>414960</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="2" t="n">
+        <v>414960</v>
+      </c>
+      <c r="B178" s="2" t="n">
+        <v>415960</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E178" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="F178" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H178" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D153" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="n">
-        <v>343960</v>
-      </c>
-      <c r="B154" s="1" t="n">
-        <v>346960</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="n">
-        <v>346960</v>
-      </c>
-      <c r="B155" s="1" t="n">
-        <v>349960</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E155" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="F155" s="1" t="s">
+    </row>
+    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="2" t="n">
+        <v>415960</v>
+      </c>
+      <c r="B179" s="2" t="n">
+        <v>418960</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F179" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="2" t="n">
+        <v>418960</v>
+      </c>
+      <c r="B180" s="2" t="n">
+        <v>420960</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="2" t="n">
+        <v>420960</v>
+      </c>
+      <c r="B181" s="2" t="n">
+        <v>423960</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="2" t="n">
+        <v>423960</v>
+      </c>
+      <c r="B182" s="2" t="n">
+        <v>425960</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="2" t="n">
+        <v>425960</v>
+      </c>
+      <c r="B183" s="2" t="n">
+        <v>431960</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="2" t="n">
+        <v>431960</v>
+      </c>
+      <c r="B184" s="2" t="n">
+        <v>433960</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="2" t="n">
+        <v>431960</v>
+      </c>
+      <c r="B185" s="2" t="n">
+        <v>433960</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E185" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="F185" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H155" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="n">
-        <v>351960</v>
-      </c>
-      <c r="B156" s="1" t="n">
-        <v>353960</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F156" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="n">
-        <v>353960</v>
-      </c>
-      <c r="B157" s="1" t="n">
-        <v>355960</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="n">
-        <v>355960</v>
-      </c>
-      <c r="B158" s="1" t="n">
-        <v>359960</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E158" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H158" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="n">
-        <v>359960</v>
-      </c>
-      <c r="B159" s="1" t="n">
-        <v>361960</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="n">
-        <v>361960</v>
-      </c>
-      <c r="B160" s="1" t="n">
-        <v>364960</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="n">
-        <v>364960</v>
-      </c>
-      <c r="B161" s="1" t="n">
-        <v>365960</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F161" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H161" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="n">
-        <v>367960</v>
-      </c>
-      <c r="B162" s="1" t="n">
-        <v>371960</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="1" t="n">
-        <v>371960</v>
-      </c>
-      <c r="B163" s="1" t="n">
-        <v>375960</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E163" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H163" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="n">
-        <v>375960</v>
-      </c>
-      <c r="B164" s="1" t="n">
-        <v>379960</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F164" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="n">
-        <v>379960</v>
-      </c>
-      <c r="B165" s="1" t="n">
-        <v>382960</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F165" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="n">
-        <v>382960</v>
-      </c>
-      <c r="B166" s="1" t="n">
-        <v>383960</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F166" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="n">
-        <v>383960</v>
-      </c>
-      <c r="B167" s="1" t="n">
-        <v>385960</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F167" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="n">
-        <v>385960</v>
-      </c>
-      <c r="B168" s="1" t="n">
-        <v>386960</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="n">
-        <v>386960</v>
-      </c>
-      <c r="B169" s="1" t="n">
-        <v>387960</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F169" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="1" t="n">
-        <v>387960</v>
-      </c>
-      <c r="B170" s="1" t="n">
-        <v>392960</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="1" t="n">
-        <v>392960</v>
-      </c>
-      <c r="B171" s="1" t="n">
-        <v>395960</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="1" t="n">
-        <v>395960</v>
-      </c>
-      <c r="B172" s="1" t="n">
-        <v>397960</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="1" t="n">
-        <v>397960</v>
-      </c>
-      <c r="B173" s="1" t="n">
-        <v>401960</v>
-      </c>
-      <c r="C173" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D173" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E173" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="F173" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H173" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="1" t="n">
-        <v>401960</v>
-      </c>
-      <c r="B174" s="1" t="n">
-        <v>404960</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F174" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="1" t="n">
-        <v>404960</v>
-      </c>
-      <c r="B175" s="1" t="n">
-        <v>407960</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D175" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F175" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="n">
-        <v>407960</v>
-      </c>
-      <c r="B176" s="1" t="n">
-        <v>410960</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="n">
-        <v>410960</v>
-      </c>
-      <c r="B177" s="1" t="n">
-        <v>414960</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D177" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="1" t="n">
-        <v>414960</v>
-      </c>
-      <c r="B178" s="1" t="n">
-        <v>415960</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E178" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="F178" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H178" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="n">
-        <v>415960</v>
-      </c>
-      <c r="B179" s="1" t="n">
-        <v>418960</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F179" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="1" t="n">
-        <v>418960</v>
-      </c>
-      <c r="B180" s="1" t="n">
-        <v>420960</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="n">
-        <v>420960</v>
-      </c>
-      <c r="B181" s="1" t="n">
-        <v>423960</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="1" t="n">
-        <v>423960</v>
-      </c>
-      <c r="B182" s="1" t="n">
-        <v>425960</v>
-      </c>
-      <c r="C182" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D182" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="1" t="n">
-        <v>425960</v>
-      </c>
-      <c r="B183" s="1" t="n">
-        <v>431960</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="1" t="n">
-        <v>431960</v>
-      </c>
-      <c r="B184" s="1" t="n">
+      <c r="H185" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="2" t="n">
         <v>433960</v>
       </c>
-      <c r="C184" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D184" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="1" t="n">
-        <v>431960</v>
-      </c>
-      <c r="B185" s="1" t="n">
-        <v>433960</v>
-      </c>
-      <c r="C185" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D185" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E185" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="F185" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H185" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="1" t="n">
-        <v>433960</v>
-      </c>
-      <c r="B186" s="1" t="n">
+      <c r="B186" s="2" t="n">
         <v>442960</v>
       </c>
-      <c r="C186" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D186" s="1" t="s">
+      <c r="C186" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D186" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="1" t="n">
+      <c r="A187" s="2" t="n">
         <v>442960</v>
       </c>
-      <c r="B187" s="1" t="n">
+      <c r="B187" s="2" t="n">
         <v>449500</v>
       </c>
-      <c r="C187" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D187" s="1" t="s">
+      <c r="C187" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D187" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="1" t="n">
+      <c r="A188" s="2" t="n">
         <v>449500</v>
       </c>
-      <c r="B188" s="1" t="n">
+      <c r="B188" s="2" t="n">
         <v>454000</v>
       </c>
-      <c r="C188" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D188" s="1" t="s">
+      <c r="C188" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D188" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>